<commit_message>
fixed commercial growers graph on excel doc
</commit_message>
<xml_diff>
--- a/topic_modeling/twitter/dist_3_graphs.xlsx
+++ b/topic_modeling/twitter/dist_3_graphs.xlsx
@@ -221,31 +221,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.242803457147</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0964535862035</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.145715415215</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.154925433813</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0121518931635</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0702164508825</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0121525622791</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25343112414</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0121500771569</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,11 +260,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2002466896"/>
-        <c:axId val="-2001946256"/>
+        <c:axId val="-1973891264"/>
+        <c:axId val="-1973841408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2002466896"/>
+        <c:axId val="-1973891264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,12 +321,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2001946256"/>
+        <c:crossAx val="-1973841408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2001946256"/>
+        <c:axId val="-1973841408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002466896"/>
+        <c:crossAx val="-1973891264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -622,11 +622,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2041656576"/>
-        <c:axId val="-1981948864"/>
+        <c:axId val="-1995255792"/>
+        <c:axId val="-1993646752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2041656576"/>
+        <c:axId val="-1995255792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,12 +683,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981948864"/>
+        <c:crossAx val="-1993646752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1981948864"/>
+        <c:axId val="-1993646752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2041656576"/>
+        <c:crossAx val="-1995255792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -989,11 +989,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1988073088"/>
-        <c:axId val="-2002432000"/>
+        <c:axId val="-2087114496"/>
+        <c:axId val="-1984836672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1988073088"/>
+        <c:axId val="-2087114496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,12 +1050,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002432000"/>
+        <c:crossAx val="-1984836672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2002432000"/>
+        <c:axId val="-1984836672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,7 +1112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988073088"/>
+        <c:crossAx val="-2087114496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1346,11 +1346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1996888176"/>
-        <c:axId val="-1990555392"/>
+        <c:axId val="-1984571264"/>
+        <c:axId val="-2018001296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1996888176"/>
+        <c:axId val="-1984571264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,12 +1407,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1990555392"/>
+        <c:crossAx val="-2018001296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1990555392"/>
+        <c:axId val="-2018001296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1996888176"/>
+        <c:crossAx val="-1984571264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1703,11 +1703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1985488096"/>
-        <c:axId val="-1981984448"/>
+        <c:axId val="-2017667984"/>
+        <c:axId val="-1991558224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1985488096"/>
+        <c:axId val="-2017667984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,12 +1764,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981984448"/>
+        <c:crossAx val="-1991558224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1981984448"/>
+        <c:axId val="-1991558224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1826,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1985488096"/>
+        <c:crossAx val="-2017667984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2065,11 +2065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1988990256"/>
-        <c:axId val="-1985359504"/>
+        <c:axId val="-1991813088"/>
+        <c:axId val="-1984117872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1988990256"/>
+        <c:axId val="-1991813088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2126,12 +2126,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1985359504"/>
+        <c:crossAx val="-1984117872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1985359504"/>
+        <c:axId val="-1984117872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2188,7 +2188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988990256"/>
+        <c:crossAx val="-1991813088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2422,11 +2422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1988896112"/>
-        <c:axId val="-1982701568"/>
+        <c:axId val="-1988266976"/>
+        <c:axId val="-2002331088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1988896112"/>
+        <c:axId val="-1988266976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2483,12 +2483,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1982701568"/>
+        <c:crossAx val="-2002331088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1982701568"/>
+        <c:axId val="-2002331088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988896112"/>
+        <c:crossAx val="-1988266976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6966,8 +6966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6980,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.242803457147</v>
+        <v>0.25</v>
       </c>
       <c r="I1">
         <v>0</v>
@@ -6994,7 +6994,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.6453586203500002E-2</v>
+        <v>0.125</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -7008,7 +7008,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.145715415215</v>
+        <v>0.125</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -7022,7 +7022,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.154925433813</v>
+        <v>0.125</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -7036,7 +7036,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1.21518931635E-2</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -7050,7 +7050,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.0216450882500003E-2</v>
+        <v>0.125</v>
       </c>
       <c r="I6">
         <v>5</v>
@@ -7064,7 +7064,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.21525622791E-2</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -7078,7 +7078,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.25343112414000002</v>
+        <v>0.25</v>
       </c>
       <c r="I8">
         <v>7</v>
@@ -7092,7 +7092,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.21500771569E-2</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>8</v>

</xml_diff>